<commit_message>
Added changes to the names of the files sent over the TLS network and file transfer results
</commit_message>
<xml_diff>
--- a/results/File_Transfer_Results.xlsx
+++ b/results/File_Transfer_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cahar\Documents\GitHub\Hybrid-Cryptography\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C826D-76FC-4DF8-8745-6F7312EF2FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211C363E-62E4-446A-B2E7-D44B7CC87709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F0E6E3B3-99E1-4FA1-860B-420909FD6595}"/>
   </bookViews>
@@ -48,6 +48,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,8 +80,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4B3E6B-87DE-463B-8FD1-0786A343E7D4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,6 +440,98 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1376</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>5254</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1568</v>
+      </c>
+      <c r="C4">
+        <f>0.946</f>
+        <v>0.94599999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3277</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>1091</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2503</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>1145</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>3265</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>2067</v>
+      </c>
+      <c r="C10" s="2">
+        <f>0.717</f>
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>1014</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <f>MEDIAN(A2:A11)</f>
+        <v>1817.5</v>
+      </c>
+      <c r="C13" s="1">
+        <f>MEDIAN(C2:C11)</f>
+        <v>1299.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>